<commit_message>
Cleaned up code after linting. Non-ASCII characters removed from test.xlsx file to avoid test failures in Windows environments.
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="PROJ" sheetId="1" state="visible" r:id="rId2"/>
@@ -65,7 +65,7 @@
     <t xml:space="preserve">123456</t>
   </si>
   <si>
-    <t xml:space="preserve">Project_Nameγ α</t>
+    <t xml:space="preserve">Project_Name</t>
   </si>
   <si>
     <t xml:space="preserve">Project_Locations</t>
@@ -532,8 +532,8 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1215,7 +1215,7 @@
   </sheetPr>
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
More tests added including to test new functionality. - Error in LLPL_PI in test_data.ags fixed - Stray data added to test.xlsx to run tests
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="PROJ" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="132">
   <si>
     <t xml:space="preserve">HEADING</t>
   </si>
@@ -363,6 +363,15 @@
   </si>
   <si>
     <t xml:space="preserve">LOCA_ENDD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEW_column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEWCOLUMN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stray_data</t>
   </si>
   <si>
     <t xml:space="preserve">Location_1</t>
@@ -532,7 +541,7 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1213,16 +1222,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="12.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1265,8 +1276,14 @@
       <c r="M1" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N1" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1285,8 +1302,11 @@
       <c r="M2" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N2" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1326,37 +1346,46 @@
       <c r="M3" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N3" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>5000000.001</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1364,31 +1393,37 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>5000000.01</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="J5" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="M5" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1396,31 +1431,37 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>5000000.1</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1428,31 +1469,170 @@
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>5000000</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="O7" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" s="0"/>
+      <c r="G8" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="N8" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="O8" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="N9" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="O9" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="O10" s="0" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix bug in dataframe_to_AGS4()
Applying the lambda function to replace double-double quotes caused
numeric data type columns to not get exported correctly. Therefore, the
string replacement is explicity applied to entries that are strings
rather that to the whole column. Test case added to verify that this
works correctly.
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="PROJ" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,7 @@
     <sheet name="TYPE" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="UNIT" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="LOCA" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="LLPL" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="149">
   <si>
     <t xml:space="preserve">HEADING</t>
   </si>
@@ -420,14 +421,66 @@
   </si>
   <si>
     <t xml:space="preserve">2019-01-21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMP_TOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMP_REF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMP_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMP_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPEC_REF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPEC_DPTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLPL_LL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLPL_PL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLPL_PI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLPL_425</t>
+  </si>
+  <si>
+    <t xml:space="preserve">327-16A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -509,7 +562,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -519,6 +572,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1224,7 +1281,7 @@
   </sheetPr>
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -1644,4 +1701,191 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>15.01</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>15.019</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>15.1234</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>15.14</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>15.1432</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>